<commit_message>
IG: phenopackets/vulcan, ref: se-genomics-2.0.0  run_id: 4017748016, run_number: 10, run_attempt: 1 with branch SHA: 0fa1b28611346e9a079c13fa18b8e6f3c3a45781 and merge SHA: ce59c317fe0f46c30a93f77fa91388a5c007962e
</commit_message>
<xml_diff>
--- a/fw-ig/core-ig-r401/pull/14_FROM_phenopackets_vulcan_se-genomics-2.0.0_TO_main/StructureDefinition-CodedOnset.xlsx
+++ b/fw-ig/core-ig-r401/pull/14_FROM_phenopackets_vulcan_se-genomics-2.0.0_TO_main/StructureDefinition-CodedOnset.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="114">
   <si>
     <t>Property</t>
   </si>
@@ -135,6 +135,9 @@
     <t>element:Condition</t>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
     <t>Path</t>
   </si>
   <si>
@@ -250,61 +253,65 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1
 </t>
   </si>
   <si>
+    <t>Extension.id</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string
+</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Extension.extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension
+</t>
+  </si>
+  <si>
+    <t>An Extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
-    <t>Extension.id</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string
-</t>
-  </si>
-  <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>Extension.extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension
-</t>
-  </si>
-  <si>
-    <t>An Extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
-  </si>
-  <si>
     <t>Extension.url</t>
   </si>
   <si>
@@ -346,6 +353,9 @@
   <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 </t>
+  </si>
+  <si>
+    <t>Extension.value[x]:valueCodeableConcept</t>
   </si>
   <si>
     <t>valueCodeableConcept</t>
@@ -669,7 +679,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ7"/>
+  <dimension ref="A1:AK7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -678,42 +688,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.59765625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="22.25390625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.95703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.77734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="16.27734375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="13.26171875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="14.4453125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="39.9765625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="19.59765625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="22.25390625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="8.95703125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.9453125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="5.4296875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="37.17578125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="17.24609375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="15.26953125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="15.6640625" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="17.171875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="19.03515625" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="18.859375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="21.57421875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="53.30078125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="22.71875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="42.03515625" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="17.21484375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="18.1875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="11.0390625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="13.875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="9.953125" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="17.171875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="21.57421875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="53.30078125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="18.1875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="11.0390625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="24.98046875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="24.98046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -825,93 +835,96 @@
       <c r="AJ1" t="s" s="1">
         <v>75</v>
       </c>
+      <c r="AK1" t="s" s="1">
+        <v>76</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
         <v>31</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>77</v>
-      </c>
+      <c r="B2" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E2" s="2"/>
       <c r="F2" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K2" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="L2" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="L2" t="s" s="2">
+      <c r="M2" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-      <c r="O2" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" t="s" s="2">
-        <v>76</v>
-      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q2" s="2"/>
       <c r="R2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="S2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="T2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="U2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="V2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="W2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="X2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Y2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Z2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AA2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AB2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AC2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AD2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AE2" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF2" t="s" s="2">
         <v>31</v>
-      </c>
-      <c r="AF2" t="s" s="2">
-        <v>77</v>
       </c>
       <c r="AG2" t="s" s="2">
         <v>78</v>
@@ -920,38 +933,41 @@
         <v>79</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
+      </c>
+      <c r="AK2" t="s" s="2">
+        <v>77</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" t="s" s="2">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E3" s="2"/>
       <c r="F3" t="s" s="2">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K3" t="s" s="2">
         <v>84</v>
@@ -959,471 +975,486 @@
       <c r="L3" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="M3" s="2"/>
+      <c r="M3" t="s" s="2">
+        <v>86</v>
+      </c>
       <c r="N3" s="2"/>
-      <c r="O3" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" t="s" s="2">
-        <v>76</v>
-      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q3" s="2"/>
       <c r="R3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="S3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="T3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="U3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="V3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="W3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="X3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Y3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Z3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AA3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AB3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AC3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AD3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="AI3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
+      </c>
+      <c r="AK3" t="s" s="2">
+        <v>88</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" t="s" s="2">
-        <v>77</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E4" s="2"/>
       <c r="F4" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="K4" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="L4" t="s" s="2">
         <v>31</v>
       </c>
-      <c r="L4" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="M4" s="2"/>
+      <c r="M4" t="s" s="2">
+        <v>91</v>
+      </c>
       <c r="N4" s="2"/>
-      <c r="O4" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" t="s" s="2">
-        <v>76</v>
-      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q4" s="2"/>
       <c r="R4" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="S4" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="T4" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="U4" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="V4" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="W4" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="X4" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Y4" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Z4" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="AB4" t="s" s="2">
         <v>92</v>
       </c>
       <c r="AC4" t="s" s="2">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="AE4" t="s" s="2">
         <v>94</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="AG4" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>76</v>
+        <v>96</v>
+      </c>
+      <c r="AK4" t="s" s="2">
+        <v>77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" t="s" s="2">
-        <v>82</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E5" s="2"/>
       <c r="F5" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="K5" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="L5" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="M5" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="N5" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q5" s="2"/>
+      <c r="R5" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="S5" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T5" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U5" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V5" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W5" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X5" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y5" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z5" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA5" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB5" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC5" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD5" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE5" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF5" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="L5" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="M5" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="N5" s="2"/>
-      <c r="O5" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="P5" s="2"/>
-      <c r="Q5" t="s" s="2">
-        <v>3</v>
-      </c>
-      <c r="R5" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S5" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T5" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U5" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V5" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W5" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X5" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y5" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z5" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA5" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB5" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC5" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD5" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE5" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="AF5" t="s" s="2">
-        <v>82</v>
-      </c>
       <c r="AG5" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>100</v>
+        <v>77</v>
+      </c>
+      <c r="AK5" t="s" s="2">
+        <v>102</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" t="s" s="2">
-        <v>77</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E6" s="2"/>
       <c r="F6" t="s" s="2">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="K6" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L6" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="M6" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q6" s="2"/>
+      <c r="R6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB6" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="AC6" s="2"/>
+      <c r="AD6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE6" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="AF6" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AG6" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH6" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AI6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ6" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="AK6" t="s" s="2">
         <v>102</v>
-      </c>
-      <c r="K6" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="L6" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="P6" s="2"/>
-      <c r="Q6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="R6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA6" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="AB6" s="2"/>
-      <c r="AC6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD6" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="AE6" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="AF6" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AG6" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AH6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AI6" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="AJ6" t="s" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" t="s" s="2">
-        <v>77</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E7" s="2"/>
       <c r="F7" t="s" s="2">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="H7" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I7" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="K7" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L7" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="M7" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q7" s="2"/>
+      <c r="R7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X7" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="Y7" s="2"/>
+      <c r="Z7" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="AA7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF7" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AG7" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH7" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AI7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ7" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="AK7" t="s" s="2">
         <v>102</v>
-      </c>
-      <c r="K7" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="L7" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="R7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W7" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="X7" s="2"/>
-      <c r="Y7" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="Z7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE7" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="AF7" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AG7" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AH7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AI7" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="AJ7" t="s" s="2">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>